<commit_message>
correct year & new songs
</commit_message>
<xml_diff>
--- a/data/genius_Kollegah_Hoodtape-volume-2.xlsx
+++ b/data/genius_Kollegah_Hoodtape-volume-2.xlsx
@@ -402,7 +402,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -468,14 +468,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -493,7 +493,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -558,14 +558,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -583,7 +583,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -626,14 +626,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -651,7 +651,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -706,14 +706,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -731,7 +731,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -802,14 +802,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -827,7 +827,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -886,14 +886,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -911,7 +911,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -991,14 +991,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1067,14 +1067,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -1092,7 +1092,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1164,14 +1164,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -1189,7 +1189,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1242,14 +1242,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -1267,7 +1267,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1303,14 +1303,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -1328,7 +1328,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1381,14 +1381,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -1406,7 +1406,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1459,14 +1459,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -1484,7 +1484,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1530,14 +1530,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -1555,7 +1555,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1613,14 +1613,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1699,14 +1699,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -1724,7 +1724,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1775,14 +1775,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -1800,7 +1800,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1864,14 +1864,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -1889,7 +1889,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1992,14 +1992,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -2017,7 +2017,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -2096,14 +2096,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -2121,7 +2121,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2210,14 +2210,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -2235,7 +2235,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2316,14 +2316,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -2341,7 +2341,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2395,14 +2395,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -2420,7 +2420,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2472,14 +2472,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2580,14 +2580,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -2605,7 +2605,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2671,14 +2671,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -2696,7 +2696,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2723,8 +2723,7 @@
 Und Warenhäuser plündernde Arme, stark das Tageslicht scheuende Straßenräuber jagen
 Manch einer schläft schutzlos unter
 Freiem Himmel, manch einer bietet seine Luxusklunker für 'nen Platz im Luftschutzbunker
-Man tauscht Gegenstände wie Eheringe und Goldketten
-Für Medizin, wesentliche Lebensmittel und Wolldecken
+Man tauscht Gegenstände wie Eheringe und GoldkettenFür Medizin, wesentliche Lebensmittel und Wolldecken
 Ein Rest Elektrizität an Notstromaggregaten
 Oder Akkus aus Technikgeräten wie Fotoapparaten
 Bringt ein Minimum an Strom
@@ -2963,14 +2962,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>
@@ -2988,7 +2987,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Hoodtape Volume 2</t>
+          <t>Hoodtape volume 2</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -3039,14 +3038,14 @@
 Label
       Alpha Music Empire
 Producers
-      Alexis Troy, B-Case, Beatzarre &amp; 10 more
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
 Writers
-      David Ruoff, Elias Klughammer &amp; Kollegah
-Copyright ©
-      Alpha Music Empire
-Label
-      Alpha Music Empire
-Phonographic Copyright ℗
+      Alexis Troy, B-Case, Beatzarre &amp; 12 more
+Composer
+      Alexis Troy, B-Case, Beatzarre &amp; 11 more
+Copyright ©
+      Alpha Music Empire
+Label
       Alpha Music Empire</t>
         </is>
       </c>

</xml_diff>